<commit_message>
[GQA] Execução do primeiro checklist de GQA.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4635" tabRatio="892" activeTab="5"/>
@@ -14,12 +14,12 @@
     <sheet name="Teste" sheetId="9" r:id="rId5"/>
     <sheet name="Legenda" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="142">
   <si>
     <t>Plano de Estimativas</t>
   </si>
@@ -390,9 +390,6 @@
     <t>EOR</t>
   </si>
   <si>
-    <t>Parcialmente Sim</t>
-  </si>
-  <si>
     <t xml:space="preserve">Não </t>
   </si>
   <si>
@@ -411,9 +408,6 @@
     <t>Não Conformidade na atividade</t>
   </si>
   <si>
-    <t>Atividades que antendem no momento mas que ainda são executadas  e são acompanhadas e reavaliadas</t>
-  </si>
-  <si>
     <t>É analisado o impacto das mudanças aprovadas?</t>
   </si>
   <si>
@@ -421,6 +415,36 @@
   </si>
   <si>
     <t>O processo é medido?</t>
+  </si>
+  <si>
+    <t>Fora da data de avaliação</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>A auditoria programada pro primeiro sprit não foi relizada na data estimada.</t>
+  </si>
+  <si>
+    <t>Algumas atividades não foram entregues no prazo.</t>
+  </si>
+  <si>
+    <t>Os casos de teste não foram definidos conforme as datas estabelecidas.</t>
+  </si>
+  <si>
+    <t>Os casos de teste não foram executados conforme as datas estabelecidas.</t>
+  </si>
+  <si>
+    <t>O plano de teste não foi entregue na datas estabelecida.</t>
+  </si>
+  <si>
+    <t>O relatório de verificação e validação dos requisitos não foi entregue.</t>
+  </si>
+  <si>
+    <t>Não tem como avaliar</t>
   </si>
 </sst>
 </file>
@@ -495,7 +519,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +547,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -555,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -566,9 +596,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -585,33 +612,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -622,7 +622,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -996,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1009,246 +1047,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.1" customHeight="1">
-      <c r="A1" s="10"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="15" t="s">
         <v>16</v>
       </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
+      <c r="B16" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
+      <c r="B17" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="24" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
+      <c r="B19" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
+      <c r="B20" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
+      <c r="B22" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
+      <c r="B23" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
+      <c r="B26" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="2" t="s">
+      <c r="B27" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="B38" s="23"/>
+      <c r="C37" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1265,7 +1437,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1278,177 +1450,257 @@
   <sheetData>
     <row r="1" spans="1:5" ht="35.1" customHeight="1">
       <c r="A1" s="3"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="B4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="B5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="B6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="B7" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="B9" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="B11" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="B12" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="B13" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="B14" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="2" t="s">
+      <c r="B18" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="5" t="s">
+      <c r="B19" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="2" t="s">
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="5" t="s">
+      <c r="B22" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" ht="30.75">
-      <c r="A24" s="13" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:4" ht="30.75">
+      <c r="A24" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="B25" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1464,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1477,304 +1729,433 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.1" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="B4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="B5" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="B6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="B7" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="B9" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="B10" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="B12" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="B13" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="B14" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="B15" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="5" t="s">
+      <c r="B16" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="14" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="14" t="s">
+      <c r="B18" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" ht="30.75">
-      <c r="A20" s="13" t="s">
+      <c r="B19" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+    </row>
+    <row r="20" spans="1:4" ht="30.75">
+      <c r="A20" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="14" t="s">
+      <c r="B20" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="2" t="s">
+      <c r="B21" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="15" t="s">
+      <c r="B22" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="5" t="s">
+      <c r="B23" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="14" t="s">
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="16" t="s">
+      <c r="B25" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" ht="30.75">
-      <c r="A27" s="16" t="s">
+      <c r="B26" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:4" ht="30.75">
+      <c r="A27" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" ht="30.75">
-      <c r="A28" s="16" t="s">
+      <c r="B27" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:4" ht="30.75">
+      <c r="A28" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" ht="30.75">
-      <c r="A29" s="16" t="s">
+      <c r="B28" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="29" spans="1:4" ht="30.75">
+      <c r="A29" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" ht="30.75">
-      <c r="A30" s="16" t="s">
+      <c r="B29" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+    </row>
+    <row r="30" spans="1:4" ht="30.75">
+      <c r="A30" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="15" t="s">
+      <c r="B30" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="5" t="s">
+      <c r="B31" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="14" t="s">
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="14" t="s">
+      <c r="B33" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" ht="30.75">
-      <c r="A35" s="16" t="s">
+      <c r="B34" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+    </row>
+    <row r="35" spans="1:4" ht="30.75">
+      <c r="A35" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" ht="30.75">
-      <c r="A36" s="16" t="s">
+      <c r="B35" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+    </row>
+    <row r="36" spans="1:4" ht="30.75">
+      <c r="A36" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="15" t="s">
+      <c r="B36" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="5" t="s">
+      <c r="B37" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="2" t="s">
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="2" t="s">
+      <c r="B39" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="1:3" ht="30.75">
-      <c r="A41" s="13" t="s">
+      <c r="B40" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17"/>
+    </row>
+    <row r="41" spans="1:4" ht="30.75">
+      <c r="A41" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="2" t="s">
+      <c r="B41" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="17"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="2" t="s">
+      <c r="B42" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="3"/>
+      <c r="B43" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1791,7 +2172,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1803,73 +2184,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.1" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="15" t="s">
         <v>47</v>
       </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="15" t="s">
         <v>49</v>
       </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="15" t="s">
         <v>51</v>
       </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -1886,7 +2295,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1898,95 +2307,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.1" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="B4" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4" ht="30.75">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" ht="30.75">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4" ht="30.75">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:4" ht="30.75">
-      <c r="A13" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C13" s="3"/>
+      <c r="A13" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -2002,7 +2443,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2011,35 +2454,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="45.75">
-      <c r="A2" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="A2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30.75">
+      <c r="A3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="75.75">
+      <c r="A4" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="30.75">
-      <c r="A3" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="90.75">
-      <c r="A4" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="75.75">
-      <c r="A5" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>128</v>
+    <row r="5" spans="1:2" ht="15.75">
+      <c r="A5" s="28"/>
+      <c r="B5" s="11" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GQA] Adição dos relatórios de não conformidades.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4635" tabRatio="892" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4635" tabRatio="892" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Processo" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Teste" sheetId="9" r:id="rId5"/>
     <sheet name="Legenda" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -426,25 +426,25 @@
     <t>Baixa</t>
   </si>
   <si>
-    <t>A auditoria programada pro primeiro sprit não foi relizada na data estimada.</t>
-  </si>
-  <si>
     <t>Algumas atividades não foram entregues no prazo.</t>
   </si>
   <si>
-    <t>Os casos de teste não foram definidos conforme as datas estabelecidas.</t>
-  </si>
-  <si>
-    <t>Os casos de teste não foram executados conforme as datas estabelecidas.</t>
-  </si>
-  <si>
-    <t>O plano de teste não foi entregue na datas estabelecida.</t>
-  </si>
-  <si>
     <t>O relatório de verificação e validação dos requisitos não foi entregue.</t>
   </si>
   <si>
     <t>Não tem como avaliar</t>
+  </si>
+  <si>
+    <t>O plano de teste não foi entregue na data estabelecida.</t>
+  </si>
+  <si>
+    <t>Os casos de teste para o Sprint 1 não foram definidos conforme as datas estabelecidas.</t>
+  </si>
+  <si>
+    <t>Os casos de teste para o Sprint 1 não foram executados conforme as datas estabelecidas.</t>
+  </si>
+  <si>
+    <t>A auditoria de configuração programada pro Sprint 1 não foi relizada na data estimada.</t>
   </si>
 </sst>
 </file>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1405,7 +1405,7 @@
       <c r="C36" s="16"/>
       <c r="D36" s="17"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="30.75">
       <c r="A37" s="17" t="s">
         <v>102</v>
       </c>
@@ -1415,8 +1415,8 @@
       <c r="C37" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D37" s="17" t="s">
-        <v>135</v>
+      <c r="D37" s="19" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1639,7 +1639,7 @@
         <v>134</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1716,8 +1716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2172,7 +2172,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" activeCellId="2" sqref="B2 C2 D2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2252,7 +2252,7 @@
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="30.75">
       <c r="A8" s="17" t="s">
         <v>52</v>
       </c>
@@ -2262,11 +2262,11 @@
       <c r="C8" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D8" s="17" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30.75">
       <c r="A9" s="17" t="s">
         <v>53</v>
       </c>
@@ -2276,8 +2276,8 @@
       <c r="C9" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>138</v>
+      <c r="D9" s="19" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2295,7 +2295,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2346,7 +2346,7 @@
         <v>134</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2426,7 +2426,7 @@
         <v>134</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2443,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2480,7 +2480,7 @@
     <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="28"/>
       <c r="B5" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GQA] Correção dos relatórios de NC.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4635" tabRatio="892" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4635" tabRatio="892" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Processo" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="140">
   <si>
     <t>Plano de Estimativas</t>
   </si>
@@ -424,12 +424,6 @@
   </si>
   <si>
     <t>Baixa</t>
-  </si>
-  <si>
-    <t>Algumas atividades não foram entregues no prazo.</t>
-  </si>
-  <si>
-    <t>O relatório de verificação e validação dos requisitos não foi entregue.</t>
   </si>
   <si>
     <t>Não tem como avaliar</t>
@@ -585,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -657,10 +651,13 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,7 +1031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -1240,7 +1237,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
@@ -1416,7 +1413,7 @@
         <v>134</v>
       </c>
       <c r="D37" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1633,14 +1630,10 @@
         <v>40</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>135</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="14" t="s">
@@ -1716,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -2172,7 +2165,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2263,7 +2256,7 @@
         <v>134</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30.75">
@@ -2277,7 +2270,7 @@
         <v>134</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2294,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2346,7 +2339,7 @@
         <v>134</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2411,7 +2404,9 @@
       <c r="A12" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="27"/>
+      <c r="B12" s="29" t="s">
+        <v>132</v>
+      </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
     </row>
@@ -2419,15 +2414,11 @@
       <c r="A13" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>136</v>
-      </c>
+      <c r="B13" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -2478,9 +2469,9 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75">
-      <c r="A5" s="28"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GQA] Realização do Checklist do Sprint 3.
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/7-Garantia da Qualidade/Checklist.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4635" tabRatio="892" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4635" tabRatio="892" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Processo" sheetId="5" r:id="rId1"/>
@@ -14,12 +14,12 @@
     <sheet name="Teste" sheetId="9" r:id="rId5"/>
     <sheet name="Legenda" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="141">
   <si>
     <t>Plano de Estimativas</t>
   </si>
@@ -429,16 +429,19 @@
     <t>Não tem como avaliar</t>
   </si>
   <si>
-    <t>O plano de teste não foi entregue na data estabelecida.</t>
-  </si>
-  <si>
-    <t>Os casos de teste para o Sprint 1 não foram definidos conforme as datas estabelecidas.</t>
-  </si>
-  <si>
-    <t>Os casos de teste para o Sprint 1 não foram executados conforme as datas estabelecidas.</t>
-  </si>
-  <si>
-    <t>A auditoria de configuração programada pro Sprint 1 não foi relizada na data estimada.</t>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>A funcionalidade de vizualisar as atividades em calendário não foi implementada na data estabelecida.</t>
+  </si>
+  <si>
+    <t>O caso de uso 10 não foi implementado na data estabelcida.</t>
+  </si>
+  <si>
+    <t>Os casos de teste para o Sprint 3 não foram definidos conforme as datas estabelecidas.</t>
+  </si>
+  <si>
+    <t>Os casos de teste para o Sprint 3 não foram executados conforme as datas estabelecidas.</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -647,9 +650,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1032,7 +1032,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1402,19 +1402,15 @@
       <c r="C36" s="16"/>
       <c r="D36" s="17"/>
     </row>
-    <row r="37" spans="1:4" ht="30.75">
+    <row r="37" spans="1:4">
       <c r="A37" s="17" t="s">
         <v>102</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>139</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="19"/>
     </row>
     <row r="38" spans="1:4">
       <c r="B38" s="13"/>
@@ -1433,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -1709,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2164,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2210,10 +2206,14 @@
         <v>48</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+        <v>133</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="14" t="s">
@@ -2225,15 +2225,19 @@
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="30.75">
       <c r="A6" s="17" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+        <v>133</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="14" t="s">
@@ -2256,7 +2260,7 @@
         <v>134</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30.75">
@@ -2270,7 +2274,7 @@
         <v>134</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2287,8 +2291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="76.5703125" defaultRowHeight="15.75"/>
@@ -2333,20 +2337,18 @@
         <v>95</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>136</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="26"/>
+      <c r="B5" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
     </row>
@@ -2354,7 +2356,9 @@
       <c r="A6" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
     </row>
@@ -2362,7 +2366,9 @@
       <c r="A7" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
     </row>
@@ -2370,7 +2376,9 @@
       <c r="A8" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="C8" s="16"/>
       <c r="D8" s="17"/>
     </row>
@@ -2378,7 +2386,9 @@
       <c r="A9" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
     </row>
@@ -2386,7 +2396,9 @@
       <c r="A10" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="C10" s="16"/>
       <c r="D10" s="17"/>
     </row>
@@ -2404,7 +2416,7 @@
       <c r="A12" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>132</v>
       </c>
       <c r="C12" s="16"/>
@@ -2414,7 +2426,7 @@
       <c r="A13" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>132</v>
       </c>
       <c r="C13" s="16"/>
@@ -2469,7 +2481,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75">
-      <c r="A5" s="27"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="11" t="s">
         <v>135</v>
       </c>

</xml_diff>